<commit_message>
updated excel example DB
</commit_message>
<xml_diff>
--- a/images/exampleTables.xlsx
+++ b/images/exampleTables.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lkc3-admin/Documents/GitHub/psychdatascience/FDS-CourseTwo/images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lkcormack/Documents/GitHub/FDS-CourseTwo/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783BBBAB-E281-B640-8F38-2A600690B901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954FBAB0-BCF4-BF40-9CFF-D35B4846CB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{29DDDEEF-AE39-3646-861D-58D0536F7D76}"/>
+    <workbookView xWindow="380" yWindow="740" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{29DDDEEF-AE39-3646-861D-58D0536F7D76}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TablesDB" sheetId="1" r:id="rId1"/>
+    <sheet name="Single table" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
   <si>
     <t>Student ID</t>
   </si>
@@ -71,13 +73,16 @@
   </si>
   <si>
     <t>Enrolled_In</t>
+  </si>
+  <si>
+    <t>Course_Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,8 +105,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,8 +133,20 @@
         <bgColor rgb="FFD9E1F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -155,11 +180,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,6 +216,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD97A9CA-9482-DB43-9151-A10B637E4B0B}">
   <dimension ref="B4:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -713,4 +754,213 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05CE666-AD09-0545-AC11-7345EA2540D7}">
+  <dimension ref="B2:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>3</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6">
+        <v>3</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="4">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="4">
+        <v>3</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="6">
+        <v>3</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="5">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>4</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="4">
+        <v>4</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="5">
+        <v>4</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="4">
+        <v>4</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6">
+        <v>4</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8B7AF6-0E78-814F-9941-C83B1526A74C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>